<commit_message>
Updated USA model - 2025-08-15 02:13
</commit_message>
<xml_diff>
--- a/VerveStacks_USA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_USA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_USA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86464818-41CF-4951-B090-313CFCBE6D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAED8889-719A-4198-8146-B79C8F557457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="misc" sheetId="7" r:id="rId1"/>
@@ -941,16 +941,16 @@
     <t>wind resource -- CF class won-USA_51 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-USA_50_c2</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-USA_50 -- cost class 2</t>
+  </si>
+  <si>
     <t>e_won-USA_50_c1</t>
   </si>
   <si>
     <t>wind resource -- CF class won-USA_50 -- cost class 1</t>
-  </si>
-  <si>
-    <t>e_won-USA_50_c2</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-USA_50 -- cost class 2</t>
   </si>
   <si>
     <t>e_won-USA_48_c1</t>
@@ -2436,7 +2436,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95316BFD-78EE-FD18-91CB-286FCE5690D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43869315-5465-2B99-05D9-D26ADFD833D4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2491,7 +2491,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0D65E8C-7E19-B66B-B2FA-44089A74C0F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92D6C9F3-B8F8-62D0-8CA8-81E2BAD9A415}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2546,7 +2546,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7396A61E-0AE8-7DAB-33AF-B14BA73936AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7268AD28-26F3-7001-120F-370145951261}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2601,7 +2601,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5F7EF1C-F62D-FF72-A74D-89B8EEEA11AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC13F070-8518-CCEA-6CEE-D6B6D8CEA704}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5104,7 +5104,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E5D01BA-D46C-4075-A437-D349DC5440B3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD03B2C1-7BC2-4186-B46D-B0764128E150}">
   <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8067,7 +8067,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE021BDD-5971-4BF9-9143-A30DB75534F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51913AB-0013-40F3-A768-5B709DF32D2C}">
   <dimension ref="A1:P178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8229,7 +8229,7 @@
         <v>18.312110612889164</v>
       </c>
       <c r="P5" s="37">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -8270,7 +8270,7 @@
         <v>18.312110612889164</v>
       </c>
       <c r="P6" s="35">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -15335,7 +15335,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE23E5ED-B0D2-4FD6-96B3-8C916724B0FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{763C0463-A27A-47F0-9B4D-239B192BACD8}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>